<commit_message>
add simple example of h5py syntax
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\alh\PycharmProjects\WPB_HDF5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432F9418-CA71-498A-B23D-88467A965BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D8C504-9365-4F03-BBEA-92DA3ACF2068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="525" windowWidth="29040" windowHeight="15720" xr2:uid="{4161688A-6E45-425F-B182-B429B9405D8C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{4161688A-6E45-425F-B182-B429B9405D8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,11 +107,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -143,62 +147,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Relative performance (%)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -701,6 +650,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Relative performance (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3889,16 +3893,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>227647</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>149542</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>532447</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>164782</xdr:rowOff>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>46673</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3925,16 +3929,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>24765</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>146685</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4301,11 +4305,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9599DD77-0471-44CA-B5F3-F2B23142E48D}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="12" max="12" width="8.88671875" style="3"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -4341,7 +4348,7 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -4382,7 +4389,7 @@
         <f t="shared" ref="K2:K8" si="0">100*H2/E2</f>
         <v>8.1337047353760443</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="3">
         <f t="shared" ref="L2:L8" si="1">100*I2/F2</f>
         <v>32.653061224489797</v>
       </c>
@@ -4424,7 +4431,7 @@
         <f t="shared" si="0"/>
         <v>157.51525235718248</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="3">
         <f t="shared" si="1"/>
         <v>25.316455696202532</v>
       </c>
@@ -4466,7 +4473,7 @@
         <f t="shared" si="0"/>
         <v>5.1959277756434892</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="3">
         <f t="shared" si="1"/>
         <v>32.653061224489797</v>
       </c>
@@ -4508,7 +4515,7 @@
         <f t="shared" si="0"/>
         <v>35.480464625131994</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="3">
         <f t="shared" si="1"/>
         <v>31.372549019607842</v>
       </c>
@@ -4550,7 +4557,7 @@
         <f t="shared" si="0"/>
         <v>3.6649987789016931</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="3">
         <f t="shared" si="1"/>
         <v>31.875</v>
       </c>
@@ -4592,7 +4599,7 @@
         <f t="shared" si="0"/>
         <v>7.1942532753196966</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="3">
         <f t="shared" si="1"/>
         <v>31.492842535787322</v>
       </c>
@@ -4634,7 +4641,7 @@
         <f t="shared" si="0"/>
         <v>272.05660264190527</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="3">
         <f t="shared" si="1"/>
         <v>13.179487179487179</v>
       </c>
@@ -4676,7 +4683,7 @@
         <f>100*H9/E9</f>
         <v>5.0621875749673801</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="3">
         <f>100*I9/F9</f>
         <v>30.6</v>
       </c>
@@ -4718,7 +4725,7 @@
         <f>100*H10/E10</f>
         <v>243.84967057161163</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="3">
         <f>100*I10/F10</f>
         <v>21.153846153846153</v>
       </c>

</xml_diff>